<commit_message>
Refined with Janice, integrated with her summer vacation homework plan.
</commit_message>
<xml_diff>
--- a/暑假计划.xlsx
+++ b/暑假计划.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9135" tabRatio="736" firstSheet="8" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9135" tabRatio="736" firstSheet="8" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="贝妞愿望" sheetId="5" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="贝妞问题诊断" sheetId="11" r:id="rId15"/>
     <sheet name="目标大表" sheetId="14" r:id="rId16"/>
     <sheet name="文件表" sheetId="19" r:id="rId17"/>
+    <sheet name="周计划" sheetId="20" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="10">'项目-编程'!$A$1:$I$15</definedName>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="513">
   <si>
     <t>数学</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1003,10 +1004,6 @@
   </si>
   <si>
     <t>学员签字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>监管者签字</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1572,22 +1569,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>数学错题本（放假前考试不及格，最后考试，加上暑期所有错题）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>项目-数学</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>项目-数学</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>全优课堂对应练习</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>编程目标-2</t>
   </si>
   <si>
@@ -1662,22 +1643,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>七年级数学上册</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>七年级数学下册</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>七年级英语上册</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>七年级英语下册</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>草稿本</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1731,10 +1696,6 @@
   </si>
   <si>
     <t>是。监督员阅读并签字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是。完成对应的章节学习和练习</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1821,6 +1782,289 @@
   </si>
   <si>
     <t>观看《厉害了我的国》</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16开，10张《长征》读后日记</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>整理文集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是。不少于15篇的大作文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>整体</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>监督员签字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英语1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读三本英文书</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英语2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读报纸《Teens》5期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英语2（2期）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英语2（3期）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英语3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英语4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英语3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英语4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《盒子鱼》（手机）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英语5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语文1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语文2</t>
+  </si>
+  <si>
+    <t>语文3</t>
+  </si>
+  <si>
+    <t>语文1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用A4田格纸抄写并背诵语文古诗（共21首）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>朗读打卡（手机）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抄写M1-M5课文，及单词表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二周打卡（83,85,87）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学2</t>
+  </si>
+  <si>
+    <t>第三周打卡（91,92,95,96,99）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学3</t>
+  </si>
+  <si>
+    <t>第四周打卡（100,102,108，111）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学4</t>
+  </si>
+  <si>
+    <t>历史1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>游览名山大川，准备A4纸做一个手抄报</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地理1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>写个PPT，图加文，自然地理特色和地方文化特色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英语口语1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一周打卡（39-45，51）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是。全优课堂对应练习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物理1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>科技馆参观学习提纲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生物1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暑假作业一张</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>道法1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>体育1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每天跑步至少1KM（五分钟以内），垫排球500次，仰卧起坐（Week29,30，每天50个；其他星期每天100个）；游泳1KM，30分钟以内。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>否。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自定-数学1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学错题本（放假前考试不及格，最后考试，共三份卷子）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自定-数学2</t>
+  </si>
+  <si>
+    <t>做7年级数学卷子，针对弱点加强学习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自定-数学3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>做8年级上数学卷子，针对弱加强学习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自定-英语1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新东方单词速记大全每天5个单元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自定-英语1（从第30周起）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物理2</t>
+  </si>
+  <si>
+    <t>物理3</t>
+  </si>
+  <si>
+    <t>道法2</t>
+  </si>
+  <si>
+    <t>看《厉害了我的国》，交A3手抄报</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>写时事PPT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载物理书并预习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物理2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三个物理实践活动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vacation Memory Book</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2822,7 +3066,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3222,6 +3466,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3234,12 +3493,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3261,15 +3514,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3311,6 +3555,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3658,7 +3905,7 @@
         <v>203</v>
       </c>
       <c r="B8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -3673,7 +3920,7 @@
   <dimension ref="B1:H31"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3690,24 +3937,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45.4" customHeight="1" thickBot="1">
-      <c r="B1" s="135" t="s">
-        <v>345</v>
-      </c>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
+      <c r="B1" s="140" t="s">
+        <v>344</v>
+      </c>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
     </row>
     <row r="2" spans="2:8">
       <c r="B2" s="34" t="s">
-        <v>255</v>
-      </c>
-      <c r="C2" s="141" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2" s="144" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="142"/>
+      <c r="D2" s="145"/>
       <c r="E2" s="53" t="s">
         <v>204</v>
       </c>
@@ -3725,285 +3972,285 @@
       <c r="B3" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="143" t="s">
+      <c r="C3" s="146" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="133"/>
+      <c r="D3" s="138"/>
       <c r="E3" s="82"/>
       <c r="F3" s="78" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G3" s="77"/>
       <c r="H3" s="81" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="133" t="s">
-        <v>247</v>
-      </c>
-      <c r="D4" s="133"/>
-      <c r="E4" s="133"/>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
-      <c r="H4" s="134"/>
+      <c r="C4" s="138" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="139"/>
     </row>
     <row r="5" spans="2:8" ht="69" customHeight="1">
       <c r="B5" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="C5" s="139" t="s">
-        <v>276</v>
-      </c>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="140"/>
+      <c r="C5" s="142" t="s">
+        <v>275</v>
+      </c>
+      <c r="D5" s="142"/>
+      <c r="E5" s="142"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="142"/>
+      <c r="H5" s="143"/>
     </row>
     <row r="6" spans="2:8" ht="45" customHeight="1">
       <c r="B6" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="139" t="s">
+      <c r="C6" s="142" t="s">
+        <v>340</v>
+      </c>
+      <c r="D6" s="142"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="143"/>
+    </row>
+    <row r="7" spans="2:8" ht="220.5" customHeight="1">
+      <c r="B7" s="135" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="142" t="s">
         <v>341</v>
       </c>
-      <c r="D6" s="139"/>
-      <c r="E6" s="139"/>
-      <c r="F6" s="139"/>
-      <c r="G6" s="139"/>
-      <c r="H6" s="140"/>
-    </row>
-    <row r="7" spans="2:8" ht="220.5" customHeight="1">
-      <c r="B7" s="146" t="s">
-        <v>158</v>
-      </c>
-      <c r="C7" s="139" t="s">
-        <v>342</v>
-      </c>
-      <c r="D7" s="144"/>
-      <c r="E7" s="144"/>
-      <c r="F7" s="144"/>
-      <c r="G7" s="144"/>
-      <c r="H7" s="145"/>
+      <c r="D7" s="147"/>
+      <c r="E7" s="147"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="148"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="147"/>
+      <c r="B8" s="136"/>
       <c r="C8" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="D8" s="137" t="s">
+      <c r="D8" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="137"/>
-      <c r="F8" s="137"/>
-      <c r="G8" s="137"/>
-      <c r="H8" s="138"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
+      <c r="H8" s="134"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="147"/>
+      <c r="B9" s="136"/>
       <c r="C9" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="D9" s="137" t="s">
+      <c r="D9" s="133" t="s">
         <v>214</v>
       </c>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="137"/>
-      <c r="H9" s="138"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="133"/>
+      <c r="H9" s="134"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="147"/>
+      <c r="B10" s="136"/>
       <c r="C10" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="D10" s="137" t="s">
+      <c r="D10" s="133" t="s">
         <v>215</v>
       </c>
-      <c r="E10" s="137"/>
-      <c r="F10" s="137"/>
-      <c r="G10" s="137"/>
-      <c r="H10" s="138"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="133"/>
+      <c r="G10" s="133"/>
+      <c r="H10" s="134"/>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="147"/>
+      <c r="B11" s="136"/>
       <c r="C11" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="D11" s="137" t="s">
-        <v>280</v>
-      </c>
-      <c r="E11" s="137"/>
-      <c r="F11" s="137"/>
-      <c r="G11" s="137"/>
-      <c r="H11" s="138"/>
+      <c r="D11" s="133" t="s">
+        <v>279</v>
+      </c>
+      <c r="E11" s="133"/>
+      <c r="F11" s="133"/>
+      <c r="G11" s="133"/>
+      <c r="H11" s="134"/>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="147"/>
+      <c r="B12" s="136"/>
       <c r="C12" s="24" t="s">
         <v>227</v>
       </c>
-      <c r="D12" s="137" t="s">
-        <v>281</v>
-      </c>
-      <c r="E12" s="137"/>
-      <c r="F12" s="137"/>
-      <c r="G12" s="137"/>
-      <c r="H12" s="138"/>
+      <c r="D12" s="133" t="s">
+        <v>280</v>
+      </c>
+      <c r="E12" s="133"/>
+      <c r="F12" s="133"/>
+      <c r="G12" s="133"/>
+      <c r="H12" s="134"/>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="147"/>
+      <c r="B13" s="136"/>
       <c r="C13" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="D13" s="137" t="s">
+      <c r="D13" s="133" t="s">
         <v>216</v>
       </c>
-      <c r="E13" s="137"/>
-      <c r="F13" s="137"/>
-      <c r="G13" s="137"/>
-      <c r="H13" s="138"/>
+      <c r="E13" s="133"/>
+      <c r="F13" s="133"/>
+      <c r="G13" s="133"/>
+      <c r="H13" s="134"/>
     </row>
     <row r="14" spans="2:8" ht="27.4" customHeight="1">
-      <c r="B14" s="147"/>
+      <c r="B14" s="136"/>
       <c r="C14" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="D14" s="137" t="s">
+      <c r="D14" s="133" t="s">
         <v>171</v>
       </c>
-      <c r="E14" s="137"/>
-      <c r="F14" s="137"/>
-      <c r="G14" s="137"/>
-      <c r="H14" s="138"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="133"/>
+      <c r="G14" s="133"/>
+      <c r="H14" s="134"/>
     </row>
     <row r="15" spans="2:8" ht="27.75" customHeight="1">
-      <c r="B15" s="147"/>
+      <c r="B15" s="136"/>
       <c r="C15" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="D15" s="137" t="s">
+      <c r="D15" s="133" t="s">
         <v>198</v>
       </c>
-      <c r="E15" s="137"/>
-      <c r="F15" s="137"/>
-      <c r="G15" s="137"/>
-      <c r="H15" s="138"/>
+      <c r="E15" s="133"/>
+      <c r="F15" s="133"/>
+      <c r="G15" s="133"/>
+      <c r="H15" s="134"/>
     </row>
     <row r="16" spans="2:8" ht="27.4" customHeight="1">
-      <c r="B16" s="147"/>
+      <c r="B16" s="136"/>
       <c r="C16" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="D16" s="137" t="s">
+      <c r="D16" s="133" t="s">
         <v>217</v>
       </c>
-      <c r="E16" s="137"/>
-      <c r="F16" s="137"/>
-      <c r="G16" s="137"/>
-      <c r="H16" s="138"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="133"/>
+      <c r="G16" s="133"/>
+      <c r="H16" s="134"/>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="147"/>
+      <c r="B17" s="136"/>
       <c r="C17" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="D17" s="137" t="s">
+      <c r="D17" s="133" t="s">
         <v>218</v>
       </c>
-      <c r="E17" s="137"/>
-      <c r="F17" s="137"/>
-      <c r="G17" s="137"/>
-      <c r="H17" s="138"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="133"/>
+      <c r="G17" s="133"/>
+      <c r="H17" s="134"/>
     </row>
     <row r="18" spans="2:8" ht="27.4" customHeight="1">
-      <c r="B18" s="147"/>
+      <c r="B18" s="136"/>
       <c r="C18" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="D18" s="137" t="s">
+      <c r="D18" s="133" t="s">
         <v>219</v>
       </c>
-      <c r="E18" s="137"/>
-      <c r="F18" s="137"/>
-      <c r="G18" s="137"/>
-      <c r="H18" s="138"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="133"/>
+      <c r="G18" s="133"/>
+      <c r="H18" s="134"/>
     </row>
     <row r="19" spans="2:8" ht="27.75" customHeight="1">
-      <c r="B19" s="147"/>
+      <c r="B19" s="136"/>
       <c r="C19" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="D19" s="137" t="s">
+      <c r="D19" s="133" t="s">
         <v>191</v>
       </c>
-      <c r="E19" s="137"/>
-      <c r="F19" s="137"/>
-      <c r="G19" s="137"/>
-      <c r="H19" s="138"/>
+      <c r="E19" s="133"/>
+      <c r="F19" s="133"/>
+      <c r="G19" s="133"/>
+      <c r="H19" s="134"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="147"/>
+      <c r="B20" s="136"/>
       <c r="C20" s="24" t="s">
         <v>237</v>
       </c>
-      <c r="D20" s="137" t="s">
+      <c r="D20" s="133" t="s">
         <v>242</v>
       </c>
-      <c r="E20" s="137"/>
-      <c r="F20" s="137"/>
-      <c r="G20" s="137"/>
-      <c r="H20" s="138"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="133"/>
+      <c r="G20" s="133"/>
+      <c r="H20" s="134"/>
     </row>
     <row r="21" spans="2:8">
-      <c r="B21" s="147"/>
+      <c r="B21" s="136"/>
       <c r="C21" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="D21" s="137" t="s">
+      <c r="D21" s="133" t="s">
         <v>220</v>
       </c>
-      <c r="E21" s="137"/>
-      <c r="F21" s="137"/>
-      <c r="G21" s="137"/>
-      <c r="H21" s="138"/>
+      <c r="E21" s="133"/>
+      <c r="F21" s="133"/>
+      <c r="G21" s="133"/>
+      <c r="H21" s="134"/>
     </row>
     <row r="22" spans="2:8" ht="27.75" customHeight="1">
-      <c r="B22" s="147"/>
+      <c r="B22" s="136"/>
       <c r="C22" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="D22" s="137" t="s">
+      <c r="D22" s="133" t="s">
         <v>221</v>
       </c>
-      <c r="E22" s="137"/>
-      <c r="F22" s="137"/>
-      <c r="G22" s="137"/>
-      <c r="H22" s="138"/>
+      <c r="E22" s="133"/>
+      <c r="F22" s="133"/>
+      <c r="G22" s="133"/>
+      <c r="H22" s="134"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="148"/>
+      <c r="B23" s="137"/>
       <c r="C23" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="D23" s="137" t="s">
-        <v>343</v>
-      </c>
-      <c r="E23" s="137"/>
-      <c r="F23" s="137"/>
-      <c r="G23" s="137"/>
-      <c r="H23" s="138"/>
+      <c r="D23" s="133" t="s">
+        <v>342</v>
+      </c>
+      <c r="E23" s="133"/>
+      <c r="F23" s="133"/>
+      <c r="G23" s="133"/>
+      <c r="H23" s="134"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="39" t="s">
         <v>160</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
@@ -4014,7 +4261,7 @@
     <row r="25" spans="2:8">
       <c r="B25" s="80"/>
       <c r="C25" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -4025,7 +4272,7 @@
     <row r="26" spans="2:8">
       <c r="B26" s="41"/>
       <c r="C26" s="30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D26" s="31"/>
       <c r="E26" s="31"/>
@@ -4038,7 +4285,7 @@
         <v>199</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
@@ -4051,7 +4298,7 @@
     <row r="28" spans="2:8">
       <c r="B28" s="41"/>
       <c r="C28" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D28" s="31"/>
       <c r="E28" s="31"/>
@@ -4061,23 +4308,23 @@
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="39" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
       <c r="G29" s="29"/>
       <c r="H29" s="43" t="s">
-        <v>246</v>
+        <v>452</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="14.25" thickBot="1">
       <c r="B30" s="45"/>
       <c r="C30" s="46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D30" s="47"/>
       <c r="E30" s="47"/>
@@ -4087,17 +4334,27 @@
     </row>
     <row r="31" spans="2:8">
       <c r="B31" t="s">
+        <v>272</v>
+      </c>
+      <c r="C31" t="s">
         <v>273</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>274</v>
-      </c>
-      <c r="D31" t="s">
-        <v>275</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D15:H15"/>
+    <mergeCell ref="D16:H16"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C7:H7"/>
     <mergeCell ref="D20:H20"/>
     <mergeCell ref="D21:H21"/>
     <mergeCell ref="D22:H22"/>
@@ -4112,16 +4369,6 @@
     <mergeCell ref="D11:H11"/>
     <mergeCell ref="D12:H12"/>
     <mergeCell ref="D13:H13"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D15:H15"/>
-    <mergeCell ref="D16:H16"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C7:H7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4134,8 +4381,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:H6"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4152,24 +4399,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45.4" customHeight="1" thickBot="1">
-      <c r="B1" s="135" t="s">
-        <v>346</v>
-      </c>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
+      <c r="B1" s="140" t="s">
+        <v>345</v>
+      </c>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
     </row>
     <row r="2" spans="2:8">
       <c r="B2" s="34" t="s">
-        <v>255</v>
-      </c>
-      <c r="C2" s="141" t="s">
-        <v>320</v>
-      </c>
-      <c r="D2" s="142"/>
+        <v>254</v>
+      </c>
+      <c r="C2" s="144" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="145"/>
       <c r="E2" s="53" t="s">
         <v>204</v>
       </c>
@@ -4187,77 +4434,77 @@
       <c r="B3" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="143" t="s">
+      <c r="C3" s="146" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="133"/>
+      <c r="D3" s="138"/>
       <c r="E3" s="82"/>
       <c r="F3" s="78" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G3" s="77"/>
       <c r="H3" s="81" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="133" t="s">
-        <v>247</v>
-      </c>
-      <c r="D4" s="133"/>
-      <c r="E4" s="133"/>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
-      <c r="H4" s="134"/>
+      <c r="C4" s="138" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="139"/>
     </row>
     <row r="5" spans="2:8" ht="69" customHeight="1">
       <c r="B5" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="C5" s="139" t="s">
-        <v>321</v>
-      </c>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="140"/>
+      <c r="C5" s="142" t="s">
+        <v>320</v>
+      </c>
+      <c r="D5" s="142"/>
+      <c r="E5" s="142"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="142"/>
+      <c r="H5" s="143"/>
     </row>
     <row r="6" spans="2:8" ht="45" customHeight="1">
       <c r="B6" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="139" t="s">
-        <v>323</v>
-      </c>
-      <c r="D6" s="139"/>
-      <c r="E6" s="139"/>
-      <c r="F6" s="139"/>
-      <c r="G6" s="139"/>
-      <c r="H6" s="140"/>
+      <c r="C6" s="142" t="s">
+        <v>322</v>
+      </c>
+      <c r="D6" s="142"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="143"/>
     </row>
     <row r="7" spans="2:8" ht="190.5" customHeight="1">
       <c r="B7" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="139" t="s">
-        <v>344</v>
-      </c>
-      <c r="D7" s="144"/>
-      <c r="E7" s="144"/>
-      <c r="F7" s="144"/>
-      <c r="G7" s="144"/>
-      <c r="H7" s="145"/>
+      <c r="C7" s="142" t="s">
+        <v>343</v>
+      </c>
+      <c r="D7" s="147"/>
+      <c r="E7" s="147"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="148"/>
     </row>
     <row r="8" spans="2:8">
       <c r="B8" s="39" t="s">
         <v>160</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
@@ -4268,7 +4515,7 @@
     <row r="9" spans="2:8">
       <c r="B9" s="80"/>
       <c r="C9" s="26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
@@ -4279,7 +4526,7 @@
     <row r="10" spans="2:8">
       <c r="B10" s="41"/>
       <c r="C10" s="30" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="31"/>
@@ -4292,7 +4539,7 @@
         <v>199</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
@@ -4305,7 +4552,7 @@
     <row r="12" spans="2:8">
       <c r="B12" s="41"/>
       <c r="C12" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
@@ -4315,23 +4562,23 @@
     </row>
     <row r="13" spans="2:8">
       <c r="B13" s="39" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="43" t="s">
-        <v>246</v>
+        <v>452</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="14.25" thickBot="1">
       <c r="B14" s="45"/>
       <c r="C14" s="46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D14" s="47"/>
       <c r="E14" s="47"/>
@@ -4341,13 +4588,13 @@
     </row>
     <row r="15" spans="2:8">
       <c r="B15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15" t="s">
         <v>273</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>274</v>
-      </c>
-      <c r="D15" t="s">
-        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -4371,8 +4618,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4389,24 +4636,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45.4" customHeight="1" thickBot="1">
-      <c r="B1" s="135" t="s">
-        <v>442</v>
-      </c>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
+      <c r="B1" s="140" t="s">
+        <v>432</v>
+      </c>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
     </row>
     <row r="2" spans="2:8">
       <c r="B2" s="34" t="s">
-        <v>255</v>
-      </c>
-      <c r="C2" s="141" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2" s="144" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="142"/>
+      <c r="D2" s="145"/>
       <c r="E2" s="53" t="s">
         <v>204</v>
       </c>
@@ -4424,77 +4671,77 @@
       <c r="B3" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="143" t="s">
+      <c r="C3" s="146" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="133"/>
+      <c r="D3" s="138"/>
       <c r="E3" s="82"/>
       <c r="F3" s="78" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G3" s="77"/>
       <c r="H3" s="81" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="133" t="s">
-        <v>247</v>
-      </c>
-      <c r="D4" s="133"/>
-      <c r="E4" s="133"/>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
-      <c r="H4" s="134"/>
+      <c r="C4" s="138" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="139"/>
     </row>
     <row r="5" spans="2:8" ht="69" customHeight="1">
       <c r="B5" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="C5" s="139" t="s">
-        <v>434</v>
-      </c>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="140"/>
+      <c r="C5" s="142" t="s">
+        <v>424</v>
+      </c>
+      <c r="D5" s="142"/>
+      <c r="E5" s="142"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="142"/>
+      <c r="H5" s="143"/>
     </row>
     <row r="6" spans="2:8" ht="45" customHeight="1">
       <c r="B6" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="139" t="s">
-        <v>435</v>
-      </c>
-      <c r="D6" s="139"/>
-      <c r="E6" s="139"/>
-      <c r="F6" s="139"/>
-      <c r="G6" s="139"/>
-      <c r="H6" s="140"/>
+      <c r="C6" s="142" t="s">
+        <v>425</v>
+      </c>
+      <c r="D6" s="142"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="143"/>
     </row>
     <row r="7" spans="2:8" ht="180.4" customHeight="1">
       <c r="B7" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="139" t="s">
-        <v>441</v>
-      </c>
-      <c r="D7" s="144"/>
-      <c r="E7" s="144"/>
-      <c r="F7" s="144"/>
-      <c r="G7" s="144"/>
-      <c r="H7" s="145"/>
+      <c r="C7" s="142" t="s">
+        <v>431</v>
+      </c>
+      <c r="D7" s="147"/>
+      <c r="E7" s="147"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="148"/>
     </row>
     <row r="8" spans="2:8">
       <c r="B8" s="39" t="s">
         <v>160</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
@@ -4505,7 +4752,7 @@
     <row r="9" spans="2:8">
       <c r="B9" s="80"/>
       <c r="C9" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
@@ -4516,7 +4763,7 @@
     <row r="10" spans="2:8">
       <c r="B10" s="41"/>
       <c r="C10" s="30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="31"/>
@@ -4529,7 +4776,7 @@
         <v>199</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
@@ -4542,7 +4789,7 @@
     <row r="12" spans="2:8">
       <c r="B12" s="41"/>
       <c r="C12" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
@@ -4552,23 +4799,23 @@
     </row>
     <row r="13" spans="2:8">
       <c r="B13" s="39" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="43" t="s">
-        <v>246</v>
+        <v>452</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="14.25" thickBot="1">
       <c r="B14" s="45"/>
       <c r="C14" s="46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D14" s="47"/>
       <c r="E14" s="47"/>
@@ -4578,13 +4825,13 @@
     </row>
     <row r="15" spans="2:8">
       <c r="B15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15" t="s">
         <v>273</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>274</v>
-      </c>
-      <c r="D15" t="s">
-        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -4608,8 +4855,8 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4626,24 +4873,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45.4" customHeight="1" thickBot="1">
-      <c r="B1" s="135" t="s">
-        <v>348</v>
-      </c>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
+      <c r="B1" s="140" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
     </row>
     <row r="2" spans="2:8">
       <c r="B2" s="34" t="s">
-        <v>255</v>
-      </c>
-      <c r="C2" s="141" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2" s="144" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="142"/>
+      <c r="D2" s="145"/>
       <c r="E2" s="53" t="s">
         <v>204</v>
       </c>
@@ -4661,77 +4908,77 @@
       <c r="B3" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="143" t="s">
+      <c r="C3" s="146" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="133"/>
+      <c r="D3" s="138"/>
       <c r="E3" s="82"/>
       <c r="F3" s="78" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G3" s="77"/>
       <c r="H3" s="81" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="133" t="s">
-        <v>247</v>
-      </c>
-      <c r="D4" s="133"/>
-      <c r="E4" s="133"/>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
-      <c r="H4" s="134"/>
+      <c r="C4" s="138" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="139"/>
     </row>
     <row r="5" spans="2:8" ht="69" customHeight="1">
       <c r="B5" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="C5" s="139" t="s">
-        <v>337</v>
-      </c>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="140"/>
+      <c r="C5" s="142" t="s">
+        <v>336</v>
+      </c>
+      <c r="D5" s="142"/>
+      <c r="E5" s="142"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="142"/>
+      <c r="H5" s="143"/>
     </row>
     <row r="6" spans="2:8" ht="45" customHeight="1">
       <c r="B6" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="139" t="s">
-        <v>338</v>
-      </c>
-      <c r="D6" s="139"/>
-      <c r="E6" s="139"/>
-      <c r="F6" s="139"/>
-      <c r="G6" s="139"/>
-      <c r="H6" s="140"/>
+      <c r="C6" s="142" t="s">
+        <v>337</v>
+      </c>
+      <c r="D6" s="142"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="143"/>
     </row>
     <row r="7" spans="2:8" ht="180.4" customHeight="1">
       <c r="B7" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="139" t="s">
-        <v>447</v>
-      </c>
-      <c r="D7" s="144"/>
-      <c r="E7" s="144"/>
-      <c r="F7" s="144"/>
-      <c r="G7" s="144"/>
-      <c r="H7" s="145"/>
+      <c r="C7" s="142" t="s">
+        <v>437</v>
+      </c>
+      <c r="D7" s="147"/>
+      <c r="E7" s="147"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="148"/>
     </row>
     <row r="8" spans="2:8">
       <c r="B8" s="39" t="s">
         <v>160</v>
       </c>
       <c r="C8" s="88" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
@@ -4742,7 +4989,7 @@
     <row r="9" spans="2:8">
       <c r="B9" s="80"/>
       <c r="C9" s="89" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
@@ -4764,7 +5011,7 @@
         <v>199</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
@@ -4777,7 +5024,7 @@
     <row r="12" spans="2:8">
       <c r="B12" s="41"/>
       <c r="C12" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
@@ -4787,23 +5034,23 @@
     </row>
     <row r="13" spans="2:8">
       <c r="B13" s="39" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
       <c r="H13" s="43" t="s">
-        <v>246</v>
+        <v>452</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="14.25" thickBot="1">
       <c r="B14" s="45"/>
       <c r="C14" s="46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D14" s="47"/>
       <c r="E14" s="47"/>
@@ -4813,13 +5060,13 @@
     </row>
     <row r="15" spans="2:8">
       <c r="B15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15" t="s">
         <v>273</v>
       </c>
-      <c r="C15" t="s">
-        <v>274</v>
-      </c>
       <c r="D15" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -4843,8 +5090,8 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4861,24 +5108,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45.4" customHeight="1" thickBot="1">
-      <c r="B1" s="135" t="s">
-        <v>423</v>
-      </c>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
+      <c r="B1" s="140" t="s">
+        <v>414</v>
+      </c>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
     </row>
     <row r="2" spans="2:8">
       <c r="B2" s="34" t="s">
-        <v>255</v>
-      </c>
-      <c r="C2" s="141" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2" s="142"/>
+        <v>254</v>
+      </c>
+      <c r="C2" s="144" t="s">
+        <v>329</v>
+      </c>
+      <c r="D2" s="145"/>
       <c r="E2" s="53" t="s">
         <v>204</v>
       </c>
@@ -4896,62 +5143,62 @@
       <c r="B3" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="143" t="s">
+      <c r="C3" s="146" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="133"/>
+      <c r="D3" s="138"/>
       <c r="E3" s="82"/>
       <c r="F3" s="78" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G3" s="77"/>
       <c r="H3" s="81" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="133" t="s">
-        <v>247</v>
-      </c>
-      <c r="D4" s="133"/>
-      <c r="E4" s="133"/>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
-      <c r="H4" s="134"/>
+      <c r="C4" s="138" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="139"/>
     </row>
     <row r="5" spans="2:8" ht="69" customHeight="1">
       <c r="B5" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="C5" s="139" t="s">
-        <v>333</v>
-      </c>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="140"/>
+      <c r="C5" s="142" t="s">
+        <v>332</v>
+      </c>
+      <c r="D5" s="142"/>
+      <c r="E5" s="142"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="142"/>
+      <c r="H5" s="143"/>
     </row>
     <row r="6" spans="2:8" ht="45" customHeight="1">
       <c r="B6" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="139" t="s">
-        <v>334</v>
-      </c>
-      <c r="D6" s="139"/>
-      <c r="E6" s="139"/>
-      <c r="F6" s="139"/>
-      <c r="G6" s="139"/>
-      <c r="H6" s="140"/>
+      <c r="C6" s="142" t="s">
+        <v>333</v>
+      </c>
+      <c r="D6" s="142"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="143"/>
     </row>
     <row r="7" spans="2:8" ht="102.75" customHeight="1">
-      <c r="B7" s="146"/>
+      <c r="B7" s="135"/>
       <c r="C7" s="149" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D7" s="150"/>
       <c r="E7" s="150"/>
@@ -4960,27 +5207,27 @@
       <c r="H7" s="151"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="147"/>
+      <c r="B8" s="136"/>
       <c r="C8" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="D8" t="s">
         <v>371</v>
-      </c>
-      <c r="D8" t="s">
-        <v>372</v>
       </c>
       <c r="E8" s="99"/>
       <c r="F8" s="99" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G8" s="99"/>
       <c r="H8" s="100"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="147"/>
+      <c r="B9" s="136"/>
       <c r="C9" s="21" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E9" s="99"/>
       <c r="F9" s="99">
@@ -4990,12 +5237,12 @@
       <c r="H9" s="100"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="147"/>
+      <c r="B10" s="136"/>
       <c r="C10" s="21" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E10" s="99"/>
       <c r="F10" s="99">
@@ -5005,12 +5252,12 @@
       <c r="H10" s="100"/>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="147"/>
+      <c r="B11" s="136"/>
       <c r="C11" s="21" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E11" s="99"/>
       <c r="F11" s="99">
@@ -5020,12 +5267,12 @@
       <c r="H11" s="100"/>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="147"/>
+      <c r="B12" s="136"/>
       <c r="C12" s="21" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E12" s="99"/>
       <c r="F12" s="99">
@@ -5035,12 +5282,12 @@
       <c r="H12" s="100"/>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="147"/>
+      <c r="B13" s="136"/>
       <c r="C13" s="21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E13" s="99"/>
       <c r="F13" s="99">
@@ -5050,12 +5297,12 @@
       <c r="H13" s="100"/>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="147"/>
+      <c r="B14" s="136"/>
       <c r="C14" s="21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E14" s="99"/>
       <c r="F14" s="99">
@@ -5065,12 +5312,12 @@
       <c r="H14" s="100"/>
     </row>
     <row r="15" spans="2:8">
-      <c r="B15" s="147"/>
+      <c r="B15" s="136"/>
       <c r="C15" s="21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E15" s="99"/>
       <c r="F15" s="99">
@@ -5080,12 +5327,12 @@
       <c r="H15" s="100"/>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="147"/>
+      <c r="B16" s="136"/>
       <c r="C16" s="21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D16" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E16" s="99"/>
       <c r="F16" s="99">
@@ -5095,12 +5342,12 @@
       <c r="H16" s="100"/>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="147"/>
+      <c r="B17" s="136"/>
       <c r="C17" s="21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E17" s="99"/>
       <c r="F17" s="99">
@@ -5110,12 +5357,12 @@
       <c r="H17" s="100"/>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="147"/>
+      <c r="B18" s="136"/>
       <c r="C18" s="21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E18" s="99"/>
       <c r="F18" s="99">
@@ -5125,12 +5372,12 @@
       <c r="H18" s="100"/>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="147"/>
+      <c r="B19" s="136"/>
       <c r="C19" s="21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E19" s="99"/>
       <c r="F19" s="99">
@@ -5140,12 +5387,12 @@
       <c r="H19" s="100"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="147"/>
+      <c r="B20" s="136"/>
       <c r="C20" s="21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D20" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E20" s="99"/>
       <c r="F20" s="99">
@@ -5155,12 +5402,12 @@
       <c r="H20" s="100"/>
     </row>
     <row r="21" spans="2:8">
-      <c r="B21" s="147"/>
+      <c r="B21" s="136"/>
       <c r="C21" s="21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D21" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E21" s="99"/>
       <c r="F21" s="99">
@@ -5170,12 +5417,12 @@
       <c r="H21" s="100"/>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="147"/>
+      <c r="B22" s="136"/>
       <c r="C22" s="21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E22" s="99"/>
       <c r="F22" s="99">
@@ -5185,7 +5432,7 @@
       <c r="H22" s="100"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="148"/>
+      <c r="B23" s="137"/>
       <c r="C23" s="87"/>
       <c r="D23" s="101"/>
       <c r="E23" s="101"/>
@@ -5201,7 +5448,7 @@
         <v>160</v>
       </c>
       <c r="C24" s="88" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
@@ -5212,7 +5459,7 @@
     <row r="25" spans="2:8">
       <c r="B25" s="80"/>
       <c r="C25" s="89" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -5223,7 +5470,7 @@
     <row r="26" spans="2:8">
       <c r="B26" s="41"/>
       <c r="C26" s="90" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="D26" s="31"/>
       <c r="E26" s="31"/>
@@ -5236,7 +5483,7 @@
         <v>199</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
@@ -5249,7 +5496,7 @@
     <row r="28" spans="2:8">
       <c r="B28" s="41"/>
       <c r="C28" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D28" s="31"/>
       <c r="E28" s="31"/>
@@ -5259,23 +5506,23 @@
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="39" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
       <c r="G29" s="29"/>
       <c r="H29" s="43" t="s">
-        <v>246</v>
+        <v>452</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="14.25" thickBot="1">
       <c r="B30" s="45"/>
       <c r="C30" s="46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D30" s="47"/>
       <c r="E30" s="47"/>
@@ -5285,13 +5532,13 @@
     </row>
     <row r="31" spans="2:8">
       <c r="B31" t="s">
+        <v>272</v>
+      </c>
+      <c r="C31" t="s">
         <v>273</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>274</v>
-      </c>
-      <c r="D31" t="s">
-        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -5317,7 +5564,7 @@
   <dimension ref="B1:E19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5361,7 +5608,7 @@
     <row r="4" spans="2:5" ht="40.5">
       <c r="B4" s="155"/>
       <c r="C4" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>135</v>
@@ -5533,8 +5780,8 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="B1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5546,16 +5793,16 @@
   <sheetData>
     <row r="1" spans="2:11" ht="54" customHeight="1" thickBot="1">
       <c r="D1" s="105" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="15" thickTop="1" thickBot="1">
       <c r="B2" s="118" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C2" s="119"/>
       <c r="D2" s="160" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E2" s="161"/>
       <c r="F2" s="161"/>
@@ -5563,19 +5810,19 @@
       <c r="H2" s="161"/>
       <c r="I2" s="162"/>
       <c r="J2" s="120" t="s">
+        <v>284</v>
+      </c>
+      <c r="K2" s="121" t="s">
         <v>285</v>
-      </c>
-      <c r="K2" s="121" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="14.25" thickTop="1">
       <c r="B3" s="87" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="87" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E3" s="31"/>
       <c r="F3" s="31"/>
@@ -5589,11 +5836,11 @@
     </row>
     <row r="4" spans="2:11">
       <c r="B4" s="106" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C4" s="25"/>
       <c r="D4" s="106" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
@@ -5607,11 +5854,11 @@
     </row>
     <row r="5" spans="2:11">
       <c r="B5" s="106" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C5" s="25"/>
       <c r="D5" s="106" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
@@ -5625,11 +5872,11 @@
     </row>
     <row r="6" spans="2:11">
       <c r="B6" s="106" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="106" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
@@ -5643,11 +5890,11 @@
     </row>
     <row r="7" spans="2:11">
       <c r="B7" s="106" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="106" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
@@ -5661,11 +5908,11 @@
     </row>
     <row r="8" spans="2:11">
       <c r="B8" s="106" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="106" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
@@ -5679,11 +5926,11 @@
     </row>
     <row r="9" spans="2:11">
       <c r="B9" s="106" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="106" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
@@ -5697,11 +5944,11 @@
     </row>
     <row r="10" spans="2:11">
       <c r="B10" s="106" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="106" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="25"/>
@@ -5715,11 +5962,11 @@
     </row>
     <row r="11" spans="2:11">
       <c r="B11" s="106" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="106" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
@@ -5733,11 +5980,11 @@
     </row>
     <row r="12" spans="2:11">
       <c r="B12" s="106" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="106" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E12" s="25"/>
       <c r="F12" s="25"/>
@@ -5751,11 +5998,11 @@
     </row>
     <row r="13" spans="2:11">
       <c r="B13" s="106" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="106" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
@@ -5769,11 +6016,11 @@
     </row>
     <row r="14" spans="2:11">
       <c r="B14" s="106" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="106" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="25"/>
@@ -5787,11 +6034,11 @@
     </row>
     <row r="15" spans="2:11">
       <c r="B15" s="106" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="106" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="25"/>
@@ -5805,11 +6052,11 @@
     </row>
     <row r="16" spans="2:11">
       <c r="B16" s="106" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="106" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="E16" s="25"/>
       <c r="F16" s="25"/>
@@ -5823,11 +6070,11 @@
     </row>
     <row r="17" spans="2:11">
       <c r="B17" s="106" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="106" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="25"/>
@@ -5841,11 +6088,11 @@
     </row>
     <row r="18" spans="2:11">
       <c r="B18" s="106" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="106" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="25"/>
@@ -5859,11 +6106,11 @@
     </row>
     <row r="19" spans="2:11">
       <c r="B19" s="106" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="106" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="25"/>
@@ -5877,11 +6124,11 @@
     </row>
     <row r="20" spans="2:11">
       <c r="B20" s="106" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="106" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E20" s="25"/>
       <c r="F20" s="25"/>
@@ -5895,11 +6142,11 @@
     </row>
     <row r="21" spans="2:11">
       <c r="B21" s="106" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="106" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
@@ -5913,11 +6160,11 @@
     </row>
     <row r="22" spans="2:11">
       <c r="B22" s="106" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="106" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E22" s="25"/>
       <c r="F22" s="25"/>
@@ -5931,11 +6178,11 @@
     </row>
     <row r="23" spans="2:11">
       <c r="B23" s="106" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="106" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E23" s="25"/>
       <c r="F23" s="25"/>
@@ -5949,11 +6196,11 @@
     </row>
     <row r="24" spans="2:11">
       <c r="B24" s="106" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="106" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E24" s="25"/>
       <c r="F24" s="25"/>
@@ -5967,11 +6214,11 @@
     </row>
     <row r="25" spans="2:11">
       <c r="B25" s="106" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C25" s="25"/>
       <c r="D25" s="106" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="E25" s="25"/>
       <c r="F25" s="25"/>
@@ -5985,11 +6232,11 @@
     </row>
     <row r="26" spans="2:11">
       <c r="B26" s="106" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="C26" s="25"/>
       <c r="D26" s="106" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="E26" s="25"/>
       <c r="F26" s="25"/>
@@ -6003,11 +6250,11 @@
     </row>
     <row r="27" spans="2:11">
       <c r="B27" s="106" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C27" s="25"/>
       <c r="D27" s="106" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
       <c r="E27" s="25"/>
       <c r="F27" s="25"/>
@@ -6021,11 +6268,11 @@
     </row>
     <row r="28" spans="2:11">
       <c r="B28" s="106" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C28" s="25"/>
       <c r="D28" s="106" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="E28" s="25"/>
       <c r="F28" s="25"/>
@@ -6039,11 +6286,11 @@
     </row>
     <row r="29" spans="2:11">
       <c r="B29" s="106" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C29" s="25"/>
       <c r="D29" s="106" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="E29" s="25"/>
       <c r="F29" s="25"/>
@@ -6057,7 +6304,7 @@
     </row>
     <row r="30" spans="2:11">
       <c r="B30" s="106" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C30" s="25"/>
       <c r="D30" s="106"/>
@@ -6071,7 +6318,7 @@
     </row>
     <row r="31" spans="2:11">
       <c r="B31" s="106" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="C31" s="25"/>
       <c r="D31" s="106"/>
@@ -6085,7 +6332,7 @@
     </row>
     <row r="32" spans="2:11">
       <c r="B32" s="106" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="106"/>
@@ -6099,7 +6346,7 @@
     </row>
     <row r="33" spans="2:11">
       <c r="B33" s="106" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="C33" s="25"/>
       <c r="D33" s="106"/>
@@ -6113,7 +6360,7 @@
     </row>
     <row r="34" spans="2:11" ht="14.25" thickBot="1">
       <c r="B34" s="112" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C34" s="113"/>
       <c r="D34" s="112"/>
@@ -6128,12 +6375,12 @@
     <row r="35" spans="2:11" ht="14.25" thickTop="1"/>
     <row r="37" spans="2:11" ht="14.25" thickBot="1">
       <c r="B37" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="38" spans="2:11">
       <c r="C38" s="156" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D38" s="157"/>
       <c r="E38" s="50"/>
@@ -6180,7 +6427,7 @@
         <v>43303</v>
       </c>
       <c r="J40" s="56" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="41" spans="2:11">
@@ -6216,7 +6463,7 @@
         <v>43310</v>
       </c>
       <c r="J42" s="56" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="43" spans="2:11">
@@ -6252,7 +6499,7 @@
         <v>43317</v>
       </c>
       <c r="J44" s="56" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="45" spans="2:11">
@@ -6288,7 +6535,7 @@
         <v>43324</v>
       </c>
       <c r="J46" s="56" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="47" spans="2:11">
@@ -6324,7 +6571,7 @@
         <v>43331</v>
       </c>
       <c r="J48" s="56" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="49" spans="3:10">
@@ -6360,7 +6607,7 @@
         <v>43338</v>
       </c>
       <c r="J50" s="56" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="51" spans="3:10" ht="14.25" thickBot="1">
@@ -6387,319 +6634,628 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet17"/>
-  <dimension ref="A2:E32"/>
+  <dimension ref="A2:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="29.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
-        <v>426</v>
-      </c>
-      <c r="B2" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="19" t="s">
+        <v>406</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>417</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>378</v>
       </c>
-      <c r="D2" s="19" t="s">
-        <v>411</v>
-      </c>
-      <c r="E2" s="19" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="19" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>419</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19" t="s">
         <v>381</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>427</v>
-      </c>
-      <c r="E3" s="19"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19" t="s">
-        <v>380</v>
-      </c>
-      <c r="C4" s="5" t="s">
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>428</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19" t="s">
-        <v>380</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>384</v>
-      </c>
+      <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19" t="s">
-        <v>380</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>427</v>
-      </c>
+      <c r="A6" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="D6" s="19"/>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="1:5" ht="27">
-      <c r="A7" s="19"/>
+    <row r="7" spans="1:5">
+      <c r="A7" s="19" t="s">
+        <v>410</v>
+      </c>
       <c r="B7" s="19" t="s">
-        <v>387</v>
+        <v>407</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>429</v>
-      </c>
+        <v>421</v>
+      </c>
+      <c r="D7" s="19"/>
       <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="19"/>
+      <c r="A8" s="19" t="s">
+        <v>410</v>
+      </c>
       <c r="B8" s="19" t="s">
-        <v>388</v>
+        <v>408</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>430</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="D8" s="19"/>
       <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="19"/>
+      <c r="A9" s="19" t="s">
+        <v>410</v>
+      </c>
       <c r="B9" s="19" t="s">
-        <v>412</v>
-      </c>
-      <c r="C9" s="5"/>
+        <v>409</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>423</v>
+      </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19" t="s">
-        <v>413</v>
-      </c>
-      <c r="C10" s="5"/>
+      <c r="A10" s="19" t="s">
+        <v>410</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>436</v>
+      </c>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19" t="s">
-        <v>414</v>
-      </c>
-      <c r="C11" s="5"/>
+      <c r="A11" s="19" t="s">
+        <v>465</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>442</v>
+      </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19" t="s">
-        <v>415</v>
-      </c>
-      <c r="C12" s="5"/>
+      <c r="A12" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>444</v>
+      </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19" t="s">
-        <v>419</v>
+      <c r="A13" s="19" t="s">
+        <v>467</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>469</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>416</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>431</v>
-      </c>
+        <v>441</v>
+      </c>
+      <c r="D13" s="19"/>
       <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19" t="s">
-        <v>419</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>417</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>432</v>
-      </c>
+      <c r="A14" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19" t="s">
-        <v>419</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>418</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>433</v>
-      </c>
+      <c r="A15" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19" t="s">
-        <v>419</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>446</v>
-      </c>
+      <c r="A16" s="19" t="s">
+        <v>459</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="5"/>
+      <c r="A17" s="19" t="s">
+        <v>460</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="5"/>
+      <c r="A18" s="19" t="s">
+        <v>464</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="5"/>
+      <c r="A19" s="19" t="s">
+        <v>473</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>486</v>
+      </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="5"/>
+      <c r="A20" s="19" t="s">
+        <v>475</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>486</v>
+      </c>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="5"/>
+      <c r="A21" s="19" t="s">
+        <v>477</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>486</v>
+      </c>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="5"/>
+      <c r="A22" s="19" t="s">
+        <v>479</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>486</v>
+      </c>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="5"/>
+      <c r="A23" s="19" t="s">
+        <v>480</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>442</v>
+      </c>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="5"/>
+      <c r="A24" s="19" t="s">
+        <v>482</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>442</v>
+      </c>
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="5"/>
+      <c r="A25" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="C25" s="19"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="5"/>
+      <c r="A26" s="19" t="s">
+        <v>487</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="C26" s="19"/>
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="5"/>
+      <c r="A27" s="19" t="s">
+        <v>504</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="C27" s="19"/>
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="5"/>
+      <c r="A28" s="19" t="s">
+        <v>505</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="C28" s="19"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="5"/>
+      <c r="A29" s="163" t="s">
+        <v>489</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="C29" s="19"/>
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="5"/>
+      <c r="A30" s="163" t="s">
+        <v>491</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="C30" s="19"/>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="5"/>
+      <c r="A31" s="163" t="s">
+        <v>506</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="C31" s="19"/>
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="5"/>
+    <row r="32" spans="1:5" ht="40.5">
+      <c r="A32" s="163" t="s">
+        <v>492</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>494</v>
+      </c>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
+    </row>
+    <row r="33" spans="1:5" ht="27">
+      <c r="A33" s="19" t="s">
+        <v>495</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>420</v>
+      </c>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="19" t="s">
+        <v>497</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="19" t="s">
+        <v>499</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="163" t="s">
+        <v>501</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="12.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>445</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>448</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>449</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="19" t="s">
+        <v>467</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>480</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>479</v>
+      </c>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="19" t="s">
+        <v>461</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>482</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>468</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>458</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>499</v>
+      </c>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="B4" s="163" t="s">
+        <v>464</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19" t="s">
+        <v>475</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>477</v>
+      </c>
+      <c r="F4" s="163" t="s">
+        <v>506</v>
+      </c>
+      <c r="G4" s="19"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="19" t="s">
+        <v>472</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>465</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>510</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="163" t="s">
+        <v>503</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19" t="s">
+        <v>495</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>497</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19" t="s">
+        <v>473</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="163" t="s">
+        <v>491</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>487</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="19"/>
+      <c r="B8" s="163" t="s">
+        <v>489</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19" t="s">
+        <v>505</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -7746,7 +8302,7 @@
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
       <c r="G5" s="123" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H5" s="98"/>
       <c r="I5" s="97">
@@ -7888,7 +8444,7 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="122" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="97">
@@ -7907,7 +8463,7 @@
         <v>27</v>
       </c>
       <c r="N10" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O10" s="19"/>
       <c r="P10" s="19"/>
@@ -7939,7 +8495,7 @@
         <v>28</v>
       </c>
       <c r="N11" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O11" s="19"/>
       <c r="P11" s="19"/>
@@ -7955,7 +8511,7 @@
       <c r="F12" s="19"/>
       <c r="G12" s="98"/>
       <c r="H12" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I12" s="97">
         <v>0.66666666666666663</v>
@@ -7973,7 +8529,7 @@
         <v>28</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O12" s="19"/>
       <c r="P12" s="19"/>
@@ -8383,7 +8939,7 @@
         <v>27</v>
       </c>
       <c r="N24" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O24" s="19"/>
       <c r="P24" s="19"/>
@@ -8409,7 +8965,7 @@
         <v>28</v>
       </c>
       <c r="N25" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O25" s="19"/>
       <c r="P25" s="19"/>
@@ -8435,7 +8991,7 @@
         <v>28</v>
       </c>
       <c r="N26" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O26" s="19"/>
       <c r="P26" s="19"/>
@@ -8881,7 +9437,7 @@
         <v>27</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G38" s="19"/>
       <c r="H38" s="19"/>
@@ -8901,7 +9457,7 @@
         <v>27</v>
       </c>
       <c r="N38" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O38" s="19"/>
       <c r="P38" s="19"/>
@@ -8923,7 +9479,7 @@
         <v>28</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G39" s="19"/>
       <c r="H39" s="19"/>
@@ -8943,7 +9499,7 @@
         <v>28</v>
       </c>
       <c r="N39" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O39" s="19"/>
       <c r="P39" s="19"/>
@@ -8965,7 +9521,7 @@
         <v>28</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G40" s="19"/>
       <c r="H40" s="19"/>
@@ -8985,7 +9541,7 @@
         <v>28</v>
       </c>
       <c r="N40" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O40" s="19"/>
       <c r="P40" s="19"/>
@@ -9419,7 +9975,7 @@
         <v>27</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G52" s="19"/>
       <c r="H52" s="19"/>
@@ -9439,7 +9995,7 @@
         <v>27</v>
       </c>
       <c r="N52" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O52" s="19"/>
       <c r="P52" s="19"/>
@@ -9461,7 +10017,7 @@
         <v>28</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G53" s="19"/>
       <c r="H53" s="19"/>
@@ -9481,7 +10037,7 @@
         <v>28</v>
       </c>
       <c r="N53" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O53" s="19"/>
       <c r="P53" s="19"/>
@@ -9503,7 +10059,7 @@
         <v>28</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G54" s="19"/>
       <c r="H54" s="19"/>
@@ -9523,7 +10079,7 @@
         <v>28</v>
       </c>
       <c r="N54" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O54" s="19"/>
       <c r="P54" s="19"/>
@@ -9636,25 +10192,25 @@
   <sheetData>
     <row r="1" spans="2:8" ht="56.25" customHeight="1" thickBot="1">
       <c r="B1" s="71" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D1" s="66" t="s">
+        <v>260</v>
+      </c>
+      <c r="E1" s="71" t="s">
+        <v>268</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>261</v>
       </c>
-      <c r="E1" s="71" t="s">
-        <v>269</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>262</v>
-      </c>
       <c r="G1" s="131" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H1" s="131"/>
     </row>
     <row r="2" spans="2:8" ht="14.25" thickBot="1">
       <c r="B2" s="126" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C2" s="127"/>
       <c r="D2" s="128"/>
@@ -9665,10 +10221,10 @@
         <v>173</v>
       </c>
       <c r="G2" s="72" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H2" s="65" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="23.85" customHeight="1">
@@ -9676,7 +10232,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="D3" s="63"/>
       <c r="E3" s="33"/>
@@ -9689,7 +10245,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="D4" s="63"/>
       <c r="E4" s="33"/>
@@ -9804,17 +10360,17 @@
         <v>175</v>
       </c>
       <c r="C15" s="68" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D15" s="79" t="s">
         <v>176</v>
       </c>
       <c r="E15" s="129" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F15" s="130"/>
       <c r="G15" s="129" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H15" s="132"/>
     </row>
@@ -9826,7 +10382,7 @@
         <v>119</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E16" s="23"/>
       <c r="F16" s="24"/>
@@ -9871,7 +10427,7 @@
         <v>119</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="24"/>
@@ -10060,28 +10616,28 @@
     </row>
     <row r="33" spans="2:8">
       <c r="B33" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="34" spans="2:8">
       <c r="B34" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="D34" s="76" t="s">
         <v>317</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>271</v>
-      </c>
-      <c r="D34" s="76" t="s">
-        <v>318</v>
       </c>
       <c r="E34" s="24"/>
       <c r="F34" s="19" t="s">
         <v>178</v>
       </c>
       <c r="G34" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H34" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -10158,18 +10714,18 @@
     </row>
     <row r="44" spans="2:8">
       <c r="B44" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C44" s="19"/>
       <c r="F44" s="19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G44" s="19"/>
       <c r="H44" s="19"/>
     </row>
     <row r="45" spans="2:8">
       <c r="B45" s="19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C45" s="19"/>
       <c r="F45" s="19" t="s">

</xml_diff>

<commit_message>
Modified daily check sheet
</commit_message>
<xml_diff>
--- a/暑假计划.xlsx
+++ b/暑假计划.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9135" tabRatio="736" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9135" tabRatio="736" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="贝妞愿望" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="12">'项目-锻炼'!$A$1:$I$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="13">'项目-数学'!$A$1:$I$31</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="11">'项目-英语'!$A$1:$I$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="9">'项目-自我管理'!$A$1:$I$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="9">'项目-自我管理'!$A$1:$I$35</definedName>
     <definedName name="时间表">假期大时间表!$A$2:$P$57</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="529">
   <si>
     <t>数学</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2104,6 +2104,39 @@
   <si>
     <t>主动承担家务，可以酌情加分。</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZW_12</t>
+  </si>
+  <si>
+    <t>ZW_12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>养成严守时间的好习惯，不拖拉，不迟到；不浪费时间，做一件事情不开小差。</t>
+  </si>
+  <si>
+    <t>养成严守时间的好习惯，不拖拉，不迟到；不浪费时间，做一件事情不开小差。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZW_10</t>
+  </si>
+  <si>
+    <t>每天早上及其他任何场合，自觉按时起床，自己定闹钟。不得因为自己赖床耽误大家时间。</t>
+  </si>
+  <si>
+    <t>ZW_11</t>
+  </si>
+  <si>
+    <t>主动承担家务，可以酌情加分。</t>
+  </si>
+  <si>
+    <t>SX_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>做题应该尽量按顺序做，不会做的题不要轻易跳过，可以问。</t>
   </si>
 </sst>
 </file>
@@ -2205,7 +2238,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="73">
+  <borders count="74">
     <border>
       <left/>
       <right/>
@@ -3111,6 +3144,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -3120,7 +3164,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3538,6 +3582,45 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3547,45 +3630,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3627,6 +3671,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3986,10 +4042,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="B1:H34"/>
+  <dimension ref="B1:H35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView showGridLines="0" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -4006,24 +4062,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="146" t="s">
+      <c r="B1" s="141" t="s">
         <v>344</v>
       </c>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B2" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="C2" s="150" t="s">
+      <c r="C2" s="147" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="151"/>
+      <c r="D2" s="148"/>
       <c r="E2" s="53" t="s">
         <v>204</v>
       </c>
@@ -4041,10 +4097,10 @@
       <c r="B3" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="152" t="s">
+      <c r="C3" s="149" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="144"/>
+      <c r="D3" s="139"/>
       <c r="E3" s="82"/>
       <c r="F3" s="78" t="s">
         <v>277</v>
@@ -4058,173 +4114,173 @@
       <c r="B4" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="139" t="s">
         <v>246</v>
       </c>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="145"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="140"/>
     </row>
     <row r="5" spans="2:8" ht="69" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="145" t="s">
         <v>275</v>
       </c>
-      <c r="D5" s="148"/>
-      <c r="E5" s="148"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
-      <c r="H5" s="149"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="146"/>
     </row>
     <row r="6" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="145" t="s">
         <v>340</v>
       </c>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="149"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="146"/>
     </row>
     <row r="7" spans="2:8" ht="220.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="139" t="s">
+      <c r="B7" s="152" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="148" t="s">
+      <c r="C7" s="145" t="s">
         <v>341</v>
       </c>
-      <c r="D7" s="153"/>
-      <c r="E7" s="153"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="153"/>
-      <c r="H7" s="154"/>
+      <c r="D7" s="150"/>
+      <c r="E7" s="150"/>
+      <c r="F7" s="150"/>
+      <c r="G7" s="150"/>
+      <c r="H7" s="151"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B8" s="140"/>
+      <c r="B8" s="153"/>
       <c r="C8" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="D8" s="142" t="s">
+      <c r="D8" s="143" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="142"/>
-      <c r="F8" s="142"/>
-      <c r="G8" s="142"/>
-      <c r="H8" s="143"/>
+      <c r="E8" s="143"/>
+      <c r="F8" s="143"/>
+      <c r="G8" s="143"/>
+      <c r="H8" s="144"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B9" s="140"/>
+      <c r="B9" s="153"/>
       <c r="C9" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="D9" s="142" t="s">
+      <c r="D9" s="143" t="s">
         <v>214</v>
       </c>
-      <c r="E9" s="142"/>
-      <c r="F9" s="142"/>
-      <c r="G9" s="142"/>
-      <c r="H9" s="143"/>
+      <c r="E9" s="143"/>
+      <c r="F9" s="143"/>
+      <c r="G9" s="143"/>
+      <c r="H9" s="144"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B10" s="140"/>
+      <c r="B10" s="153"/>
       <c r="C10" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="D10" s="142" t="s">
+      <c r="D10" s="143" t="s">
         <v>215</v>
       </c>
-      <c r="E10" s="142"/>
-      <c r="F10" s="142"/>
-      <c r="G10" s="142"/>
-      <c r="H10" s="143"/>
+      <c r="E10" s="143"/>
+      <c r="F10" s="143"/>
+      <c r="G10" s="143"/>
+      <c r="H10" s="144"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B11" s="140"/>
+      <c r="B11" s="153"/>
       <c r="C11" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="D11" s="142" t="s">
+      <c r="D11" s="143" t="s">
         <v>279</v>
       </c>
-      <c r="E11" s="142"/>
-      <c r="F11" s="142"/>
-      <c r="G11" s="142"/>
-      <c r="H11" s="143"/>
+      <c r="E11" s="143"/>
+      <c r="F11" s="143"/>
+      <c r="G11" s="143"/>
+      <c r="H11" s="144"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B12" s="140"/>
+      <c r="B12" s="153"/>
       <c r="C12" s="24" t="s">
         <v>227</v>
       </c>
-      <c r="D12" s="142" t="s">
+      <c r="D12" s="143" t="s">
         <v>280</v>
       </c>
-      <c r="E12" s="142"/>
-      <c r="F12" s="142"/>
-      <c r="G12" s="142"/>
-      <c r="H12" s="143"/>
+      <c r="E12" s="143"/>
+      <c r="F12" s="143"/>
+      <c r="G12" s="143"/>
+      <c r="H12" s="144"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B13" s="140"/>
+      <c r="B13" s="153"/>
       <c r="C13" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="D13" s="142" t="s">
+      <c r="D13" s="143" t="s">
         <v>216</v>
       </c>
-      <c r="E13" s="142"/>
-      <c r="F13" s="142"/>
-      <c r="G13" s="142"/>
-      <c r="H13" s="143"/>
+      <c r="E13" s="143"/>
+      <c r="F13" s="143"/>
+      <c r="G13" s="143"/>
+      <c r="H13" s="144"/>
     </row>
     <row r="14" spans="2:8" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="140"/>
+      <c r="B14" s="153"/>
       <c r="C14" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="D14" s="142" t="s">
+      <c r="D14" s="143" t="s">
         <v>171</v>
       </c>
-      <c r="E14" s="142"/>
-      <c r="F14" s="142"/>
-      <c r="G14" s="142"/>
-      <c r="H14" s="143"/>
+      <c r="E14" s="143"/>
+      <c r="F14" s="143"/>
+      <c r="G14" s="143"/>
+      <c r="H14" s="144"/>
     </row>
     <row r="15" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="140"/>
+      <c r="B15" s="153"/>
       <c r="C15" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="D15" s="142" t="s">
+      <c r="D15" s="143" t="s">
         <v>198</v>
       </c>
-      <c r="E15" s="142"/>
-      <c r="F15" s="142"/>
-      <c r="G15" s="142"/>
-      <c r="H15" s="143"/>
+      <c r="E15" s="143"/>
+      <c r="F15" s="143"/>
+      <c r="G15" s="143"/>
+      <c r="H15" s="144"/>
     </row>
     <row r="16" spans="2:8" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="140"/>
+      <c r="B16" s="153"/>
       <c r="C16" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="D16" s="142" t="s">
+      <c r="D16" s="143" t="s">
         <v>217</v>
       </c>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="143"/>
+      <c r="E16" s="143"/>
+      <c r="F16" s="143"/>
+      <c r="G16" s="143"/>
+      <c r="H16" s="144"/>
     </row>
     <row r="17" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="140"/>
+      <c r="B17" s="153"/>
       <c r="C17" s="124" t="s">
         <v>513</v>
       </c>
@@ -4237,7 +4293,7 @@
       <c r="H17" s="138"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B18" s="140"/>
+      <c r="B18" s="153"/>
       <c r="C18" s="124" t="s">
         <v>517</v>
       </c>
@@ -4250,209 +4306,239 @@
       <c r="H18" s="138"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B19" s="140"/>
-      <c r="C19" s="24" t="s">
+      <c r="B19" s="153"/>
+      <c r="C19" s="124" t="s">
+        <v>520</v>
+      </c>
+      <c r="D19" s="169" t="s">
+        <v>522</v>
+      </c>
+      <c r="E19" s="170"/>
+      <c r="F19" s="170"/>
+      <c r="G19" s="170"/>
+      <c r="H19" s="171"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B20" s="153"/>
+      <c r="C20" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="D19" s="142" t="s">
+      <c r="D20" s="143" t="s">
         <v>218</v>
       </c>
-      <c r="E19" s="142"/>
-      <c r="F19" s="142"/>
-      <c r="G19" s="142"/>
-      <c r="H19" s="143"/>
-    </row>
-    <row r="20" spans="2:8" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="140"/>
-      <c r="C20" s="24" t="s">
+      <c r="E20" s="143"/>
+      <c r="F20" s="143"/>
+      <c r="G20" s="143"/>
+      <c r="H20" s="144"/>
+    </row>
+    <row r="21" spans="2:8" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="153"/>
+      <c r="C21" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="D20" s="142" t="s">
+      <c r="D21" s="143" t="s">
         <v>219</v>
       </c>
-      <c r="E20" s="142"/>
-      <c r="F20" s="142"/>
-      <c r="G20" s="142"/>
-      <c r="H20" s="143"/>
-    </row>
-    <row r="21" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="140"/>
-      <c r="C21" s="24" t="s">
+      <c r="E21" s="143"/>
+      <c r="F21" s="143"/>
+      <c r="G21" s="143"/>
+      <c r="H21" s="144"/>
+    </row>
+    <row r="22" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="153"/>
+      <c r="C22" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="D21" s="142" t="s">
+      <c r="D22" s="143" t="s">
         <v>191</v>
       </c>
-      <c r="E21" s="142"/>
-      <c r="F21" s="142"/>
-      <c r="G21" s="142"/>
-      <c r="H21" s="143"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B22" s="140"/>
-      <c r="C22" s="24" t="s">
+      <c r="E22" s="143"/>
+      <c r="F22" s="143"/>
+      <c r="G22" s="143"/>
+      <c r="H22" s="144"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B23" s="153"/>
+      <c r="C23" s="24" t="s">
         <v>237</v>
       </c>
-      <c r="D22" s="142" t="s">
+      <c r="D23" s="143" t="s">
         <v>242</v>
       </c>
-      <c r="E22" s="142"/>
-      <c r="F22" s="142"/>
-      <c r="G22" s="142"/>
-      <c r="H22" s="143"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B23" s="140"/>
-      <c r="C23" s="24" t="s">
+      <c r="E23" s="143"/>
+      <c r="F23" s="143"/>
+      <c r="G23" s="143"/>
+      <c r="H23" s="144"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B24" s="153"/>
+      <c r="C24" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="D23" s="142" t="s">
+      <c r="D24" s="143" t="s">
         <v>220</v>
       </c>
-      <c r="E23" s="142"/>
-      <c r="F23" s="142"/>
-      <c r="G23" s="142"/>
-      <c r="H23" s="143"/>
-    </row>
-    <row r="24" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="140"/>
-      <c r="C24" s="24" t="s">
+      <c r="E24" s="143"/>
+      <c r="F24" s="143"/>
+      <c r="G24" s="143"/>
+      <c r="H24" s="144"/>
+    </row>
+    <row r="25" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="153"/>
+      <c r="C25" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="D24" s="142" t="s">
+      <c r="D25" s="143" t="s">
         <v>221</v>
       </c>
-      <c r="E24" s="142"/>
-      <c r="F24" s="142"/>
-      <c r="G24" s="142"/>
-      <c r="H24" s="143"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B25" s="140"/>
-      <c r="C25" s="24" t="s">
+      <c r="E25" s="143"/>
+      <c r="F25" s="143"/>
+      <c r="G25" s="143"/>
+      <c r="H25" s="144"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B26" s="153"/>
+      <c r="C26" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="D25" s="142" t="s">
+      <c r="D26" s="143" t="s">
         <v>342</v>
       </c>
-      <c r="E25" s="142"/>
-      <c r="F25" s="142"/>
-      <c r="G25" s="142"/>
-      <c r="H25" s="143"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B26" s="141"/>
-      <c r="C26" s="123" t="s">
+      <c r="E26" s="143"/>
+      <c r="F26" s="143"/>
+      <c r="G26" s="143"/>
+      <c r="H26" s="144"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B27" s="154"/>
+      <c r="C27" s="123" t="s">
         <v>511</v>
       </c>
-      <c r="D26" s="136" t="s">
+      <c r="D27" s="136" t="s">
         <v>512</v>
       </c>
-      <c r="E26" s="137"/>
-      <c r="F26" s="137"/>
-      <c r="G26" s="137"/>
-      <c r="H26" s="138"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B27" s="39" t="s">
+      <c r="E27" s="137"/>
+      <c r="F27" s="137"/>
+      <c r="G27" s="137"/>
+      <c r="H27" s="138"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B28" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C28" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="40"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B28" s="80"/>
-      <c r="C28" s="26" t="s">
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="40"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B29" s="80"/>
+      <c r="C29" s="26" t="s">
         <v>271</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="51"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B29" s="41"/>
-      <c r="C29" s="30" t="s">
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="51"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B30" s="41"/>
+      <c r="C30" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="42"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B30" s="39" t="s">
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="42"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B31" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C31" s="27" t="s">
         <v>249</v>
       </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="43" t="s">
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="43" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B31" s="41"/>
-      <c r="C31" s="30" t="s">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B32" s="41"/>
+      <c r="C32" s="30" t="s">
         <v>250</v>
       </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="44"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B32" s="39" t="s">
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="44"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B33" s="39" t="s">
         <v>253</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C33" s="27" t="s">
         <v>251</v>
       </c>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="43" t="s">
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="43" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="45"/>
-      <c r="C33" s="46" t="s">
+    <row r="34" spans="2:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="45"/>
+      <c r="C34" s="46" t="s">
         <v>252</v>
       </c>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="49"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B34" t="s">
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="49"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B35" t="s">
         <v>272</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>273</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>274</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="28">
+    <mergeCell ref="D19:H19"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="B7:B27"/>
+    <mergeCell ref="D17:H17"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="D13:H13"/>
     <mergeCell ref="D18:H18"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="B1:H1"/>
@@ -4464,22 +4550,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C7:H7"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="B7:B26"/>
-    <mergeCell ref="D17:H17"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="D12:H12"/>
-    <mergeCell ref="D13:H13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4510,24 +4580,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="146" t="s">
+      <c r="B1" s="141" t="s">
         <v>345</v>
       </c>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B2" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="C2" s="150" t="s">
+      <c r="C2" s="147" t="s">
         <v>319</v>
       </c>
-      <c r="D2" s="151"/>
+      <c r="D2" s="148"/>
       <c r="E2" s="53" t="s">
         <v>204</v>
       </c>
@@ -4545,10 +4615,10 @@
       <c r="B3" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="152" t="s">
+      <c r="C3" s="149" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="144"/>
+      <c r="D3" s="139"/>
       <c r="E3" s="82"/>
       <c r="F3" s="78" t="s">
         <v>277</v>
@@ -4562,53 +4632,53 @@
       <c r="B4" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="139" t="s">
         <v>246</v>
       </c>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="145"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="140"/>
     </row>
     <row r="5" spans="2:8" ht="69" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="145" t="s">
         <v>320</v>
       </c>
-      <c r="D5" s="148"/>
-      <c r="E5" s="148"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
-      <c r="H5" s="149"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="146"/>
     </row>
     <row r="6" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="145" t="s">
         <v>322</v>
       </c>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="149"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="146"/>
     </row>
     <row r="7" spans="2:8" ht="190.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="148" t="s">
+      <c r="C7" s="145" t="s">
         <v>343</v>
       </c>
-      <c r="D7" s="153"/>
-      <c r="E7" s="153"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="153"/>
-      <c r="H7" s="154"/>
+      <c r="D7" s="150"/>
+      <c r="E7" s="150"/>
+      <c r="F7" s="150"/>
+      <c r="G7" s="150"/>
+      <c r="H7" s="151"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" s="39" t="s">
@@ -4747,24 +4817,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="146" t="s">
+      <c r="B1" s="141" t="s">
         <v>431</v>
       </c>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B2" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="C2" s="150" t="s">
+      <c r="C2" s="147" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="151"/>
+      <c r="D2" s="148"/>
       <c r="E2" s="53" t="s">
         <v>204</v>
       </c>
@@ -4782,10 +4852,10 @@
       <c r="B3" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="152" t="s">
+      <c r="C3" s="149" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="144"/>
+      <c r="D3" s="139"/>
       <c r="E3" s="82"/>
       <c r="F3" s="78" t="s">
         <v>277</v>
@@ -4799,53 +4869,53 @@
       <c r="B4" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="139" t="s">
         <v>246</v>
       </c>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="145"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="140"/>
     </row>
     <row r="5" spans="2:8" ht="69" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="145" t="s">
         <v>424</v>
       </c>
-      <c r="D5" s="148"/>
-      <c r="E5" s="148"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
-      <c r="H5" s="149"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="146"/>
     </row>
     <row r="6" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="145" t="s">
         <v>425</v>
       </c>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="149"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="146"/>
     </row>
     <row r="7" spans="2:8" ht="150" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="148" t="s">
+      <c r="C7" s="145" t="s">
         <v>516</v>
       </c>
-      <c r="D7" s="153"/>
-      <c r="E7" s="153"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="153"/>
-      <c r="H7" s="154"/>
+      <c r="D7" s="150"/>
+      <c r="E7" s="150"/>
+      <c r="F7" s="150"/>
+      <c r="G7" s="150"/>
+      <c r="H7" s="151"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" s="39" t="s">
@@ -4984,24 +5054,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="146" t="s">
+      <c r="B1" s="141" t="s">
         <v>347</v>
       </c>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B2" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="C2" s="150" t="s">
+      <c r="C2" s="147" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="151"/>
+      <c r="D2" s="148"/>
       <c r="E2" s="53" t="s">
         <v>204</v>
       </c>
@@ -5019,10 +5089,10 @@
       <c r="B3" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="152" t="s">
+      <c r="C3" s="149" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="144"/>
+      <c r="D3" s="139"/>
       <c r="E3" s="82"/>
       <c r="F3" s="78" t="s">
         <v>277</v>
@@ -5036,53 +5106,53 @@
       <c r="B4" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="139" t="s">
         <v>246</v>
       </c>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="145"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="140"/>
     </row>
     <row r="5" spans="2:8" ht="69" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="145" t="s">
         <v>336</v>
       </c>
-      <c r="D5" s="148"/>
-      <c r="E5" s="148"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
-      <c r="H5" s="149"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="146"/>
     </row>
     <row r="6" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="145" t="s">
         <v>337</v>
       </c>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="149"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="146"/>
     </row>
     <row r="7" spans="2:8" ht="180.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="148" t="s">
+      <c r="C7" s="145" t="s">
         <v>515</v>
       </c>
-      <c r="D7" s="153"/>
-      <c r="E7" s="153"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="153"/>
-      <c r="H7" s="154"/>
+      <c r="D7" s="150"/>
+      <c r="E7" s="150"/>
+      <c r="F7" s="150"/>
+      <c r="G7" s="150"/>
+      <c r="H7" s="151"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" s="39" t="s">
@@ -5219,24 +5289,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="146" t="s">
+      <c r="B1" s="141" t="s">
         <v>414</v>
       </c>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B2" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="C2" s="150" t="s">
+      <c r="C2" s="147" t="s">
         <v>329</v>
       </c>
-      <c r="D2" s="151"/>
+      <c r="D2" s="148"/>
       <c r="E2" s="53" t="s">
         <v>204</v>
       </c>
@@ -5254,10 +5324,10 @@
       <c r="B3" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="152" t="s">
+      <c r="C3" s="149" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="144"/>
+      <c r="D3" s="139"/>
       <c r="E3" s="82"/>
       <c r="F3" s="78" t="s">
         <v>277</v>
@@ -5271,43 +5341,43 @@
       <c r="B4" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="139" t="s">
         <v>246</v>
       </c>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="145"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="140"/>
     </row>
     <row r="5" spans="2:8" ht="69" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="145" t="s">
         <v>332</v>
       </c>
-      <c r="D5" s="148"/>
-      <c r="E5" s="148"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
-      <c r="H5" s="149"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="146"/>
     </row>
     <row r="6" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="145" t="s">
         <v>333</v>
       </c>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="149"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="146"/>
     </row>
     <row r="7" spans="2:8" ht="102.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="139"/>
+      <c r="B7" s="152"/>
       <c r="C7" s="155" t="s">
         <v>375</v>
       </c>
@@ -5318,7 +5388,7 @@
       <c r="H7" s="157"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B8" s="140"/>
+      <c r="B8" s="153"/>
       <c r="C8" s="21" t="s">
         <v>370</v>
       </c>
@@ -5333,7 +5403,7 @@
       <c r="H8" s="100"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B9" s="140"/>
+      <c r="B9" s="153"/>
       <c r="C9" s="21" t="s">
         <v>353</v>
       </c>
@@ -5348,7 +5418,7 @@
       <c r="H9" s="100"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B10" s="140"/>
+      <c r="B10" s="153"/>
       <c r="C10" s="21" t="s">
         <v>353</v>
       </c>
@@ -5363,7 +5433,7 @@
       <c r="H10" s="100"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B11" s="140"/>
+      <c r="B11" s="153"/>
       <c r="C11" s="21" t="s">
         <v>353</v>
       </c>
@@ -5378,7 +5448,7 @@
       <c r="H11" s="100"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B12" s="140"/>
+      <c r="B12" s="153"/>
       <c r="C12" s="21" t="s">
         <v>353</v>
       </c>
@@ -5393,7 +5463,7 @@
       <c r="H12" s="100"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B13" s="140"/>
+      <c r="B13" s="153"/>
       <c r="C13" s="21" t="s">
         <v>354</v>
       </c>
@@ -5408,7 +5478,7 @@
       <c r="H13" s="100"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B14" s="140"/>
+      <c r="B14" s="153"/>
       <c r="C14" s="21" t="s">
         <v>354</v>
       </c>
@@ -5423,7 +5493,7 @@
       <c r="H14" s="100"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B15" s="140"/>
+      <c r="B15" s="153"/>
       <c r="C15" s="21" t="s">
         <v>354</v>
       </c>
@@ -5438,7 +5508,7 @@
       <c r="H15" s="100"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B16" s="140"/>
+      <c r="B16" s="153"/>
       <c r="C16" s="21" t="s">
         <v>354</v>
       </c>
@@ -5453,7 +5523,7 @@
       <c r="H16" s="100"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B17" s="140"/>
+      <c r="B17" s="153"/>
       <c r="C17" s="21" t="s">
         <v>354</v>
       </c>
@@ -5468,7 +5538,7 @@
       <c r="H17" s="100"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B18" s="140"/>
+      <c r="B18" s="153"/>
       <c r="C18" s="21" t="s">
         <v>355</v>
       </c>
@@ -5483,7 +5553,7 @@
       <c r="H18" s="100"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B19" s="140"/>
+      <c r="B19" s="153"/>
       <c r="C19" s="21" t="s">
         <v>355</v>
       </c>
@@ -5498,7 +5568,7 @@
       <c r="H19" s="100"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B20" s="140"/>
+      <c r="B20" s="153"/>
       <c r="C20" s="21" t="s">
         <v>355</v>
       </c>
@@ -5513,7 +5583,7 @@
       <c r="H20" s="100"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B21" s="140"/>
+      <c r="B21" s="153"/>
       <c r="C21" s="21" t="s">
         <v>355</v>
       </c>
@@ -5528,7 +5598,7 @@
       <c r="H21" s="100"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B22" s="140"/>
+      <c r="B22" s="153"/>
       <c r="C22" s="21" t="s">
         <v>355</v>
       </c>
@@ -5543,7 +5613,7 @@
       <c r="H22" s="100"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B23" s="141"/>
+      <c r="B23" s="154"/>
       <c r="C23" s="87"/>
       <c r="D23" s="101"/>
       <c r="E23" s="101"/>
@@ -10287,10 +10357,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="B1:H45"/>
+  <dimension ref="B1:H49"/>
   <sheetViews>
-    <sheetView zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -10622,28 +10692,28 @@
     </row>
     <row r="25" spans="2:8" ht="27.75" x14ac:dyDescent="0.4">
       <c r="B25" s="55" t="s">
-        <v>232</v>
+        <v>523</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>180</v>
+        <v>119</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>184</v>
+        <v>524</v>
       </c>
       <c r="E25" s="23"/>
       <c r="F25" s="24"/>
       <c r="G25" s="23"/>
       <c r="H25" s="74"/>
     </row>
-    <row r="26" spans="2:8" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B26" s="55" t="s">
-        <v>234</v>
+        <v>525</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>180</v>
+        <v>119</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>192</v>
+        <v>526</v>
       </c>
       <c r="E26" s="23"/>
       <c r="F26" s="24"/>
@@ -10652,13 +10722,13 @@
     </row>
     <row r="27" spans="2:8" ht="27.75" x14ac:dyDescent="0.4">
       <c r="B27" s="55" t="s">
-        <v>235</v>
+        <v>519</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>180</v>
+        <v>119</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>190</v>
+        <v>521</v>
       </c>
       <c r="E27" s="23"/>
       <c r="F27" s="24"/>
@@ -10667,28 +10737,28 @@
     </row>
     <row r="28" spans="2:8" ht="27.75" x14ac:dyDescent="0.4">
       <c r="B28" s="55" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>241</v>
+        <v>184</v>
       </c>
       <c r="E28" s="23"/>
       <c r="F28" s="24"/>
       <c r="G28" s="23"/>
       <c r="H28" s="74"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:8" ht="27.75" x14ac:dyDescent="0.4">
       <c r="B29" s="55" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E29" s="23"/>
       <c r="F29" s="24"/>
@@ -10697,95 +10767,119 @@
     </row>
     <row r="30" spans="2:8" ht="27.75" x14ac:dyDescent="0.4">
       <c r="B30" s="55" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="E30" s="23"/>
       <c r="F30" s="24"/>
       <c r="G30" s="23"/>
       <c r="H30" s="74"/>
     </row>
-    <row r="31" spans="2:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="57" t="s">
+    <row r="31" spans="2:8" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="B31" s="55" t="s">
+        <v>236</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E31" s="23"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="74"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B32" s="55" t="s">
+        <v>238</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E32" s="23"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="74"/>
+    </row>
+    <row r="33" spans="2:8" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="B33" s="55" t="s">
+        <v>239</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E33" s="23"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="74"/>
+    </row>
+    <row r="34" spans="2:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="57" t="s">
         <v>240</v>
       </c>
-      <c r="C31" s="58" t="s">
+      <c r="C34" s="58" t="s">
         <v>186</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D34" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="E31" s="69"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="75"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B33" t="s">
+      <c r="E34" s="172"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="172"/>
+      <c r="H34" s="40"/>
+    </row>
+    <row r="35" spans="2:8" ht="28.15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="57" t="s">
+        <v>527</v>
+      </c>
+      <c r="C35" s="58" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>528</v>
+      </c>
+      <c r="E35" s="69"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="75"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B37" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B34" s="19" t="s">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B38" s="19" t="s">
         <v>316</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C38" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="D34" s="76" t="s">
+      <c r="D38" s="76" t="s">
         <v>317</v>
       </c>
-      <c r="E34" s="24"/>
-      <c r="F34" s="19" t="s">
+      <c r="E38" s="24"/>
+      <c r="F38" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="G34" s="19" t="s">
+      <c r="G38" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="H34" s="19" t="s">
+      <c r="H38" s="19" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="76"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B39" s="19"/>
@@ -10823,27 +10917,63 @@
       <c r="G42" s="19"/>
       <c r="H42" s="19"/>
     </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+    </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B44" s="19" t="s">
-        <v>264</v>
-      </c>
+      <c r="B44" s="19"/>
       <c r="C44" s="19"/>
-      <c r="F44" s="19" t="s">
-        <v>265</v>
-      </c>
+      <c r="D44" s="76"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="19"/>
       <c r="G44" s="19"/>
       <c r="H44" s="19"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B45" s="19" t="s">
-        <v>263</v>
-      </c>
+      <c r="B45" s="19"/>
       <c r="C45" s="19"/>
-      <c r="F45" s="19" t="s">
-        <v>177</v>
-      </c>
+      <c r="D45" s="76"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="19"/>
       <c r="G45" s="19"/>
       <c r="H45" s="19"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="76"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B48" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="C48" s="19"/>
+      <c r="F48" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B49" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="C49" s="19"/>
+      <c r="F49" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>